<commit_message>
Updated changed file names
</commit_message>
<xml_diff>
--- a/blastdb/config.xlsx
+++ b/blastdb/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sradak/Downloads/variable_extract/blastdb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563A6984-E0D8-614B-A656-AC806FD6EBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7D7CA7-6842-A34E-B58B-77F221BA3EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="10960" windowWidth="30240" windowHeight="17180" xr2:uid="{D0C1844A-0301-C241-837A-D904870A691A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17040" xr2:uid="{D0C1844A-0301-C241-837A-D904870A691A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,12 +111,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -140,8 +146,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,43 +485,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAB6C40-4C96-8C45-B281-25BF0FCB6B5C}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="186" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I1" sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
     <col min="6" max="6" width="20.1640625" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" customWidth="1"/>
     <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>